<commit_message>
by all members morning batch
</commit_message>
<xml_diff>
--- a/visog-job-portal-api/src/main/resources/Excel_Worksheet/Visog_WorkSheet1.xlsx
+++ b/visog-job-portal-api/src/main/resources/Excel_Worksheet/Visog_WorkSheet1.xlsx
@@ -12,12 +12,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="63">
   <si>
     <t>TABLE NAME</t>
   </si>
@@ -203,6 +202,9 @@
   </si>
   <si>
     <t>Bala</t>
+  </si>
+  <si>
+    <t>Login</t>
   </si>
 </sst>
 </file>
@@ -1024,10 +1026,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L36"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1689,7 +1691,7 @@
         <v>27</v>
       </c>
       <c r="C24" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D24" t="s">
         <v>49</v>
@@ -1706,7 +1708,7 @@
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="D25" t="s">
         <v>49</v>
@@ -1791,7 +1793,7 @@
         <v>24</v>
       </c>
       <c r="C30" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="D30" t="s">
         <v>49</v>
@@ -1842,7 +1844,7 @@
         <v>28</v>
       </c>
       <c r="C33" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D33" t="s">
         <v>49</v>
@@ -1900,6 +1902,11 @@
       </c>
       <c r="E36" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>